<commit_message>
docs -> notlarim junction; t├╝m notlar eklendi
</commit_message>
<xml_diff>
--- a/docs/ArchiX_Is_Takip_Listesi.xlsx
+++ b/docs/ArchiX_Is_Takip_Listesi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\ArchiX\notlarim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1585F5-E518-4829-9D7B-1BFC9A4D9A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F2C14E-7F6E-4FF9-A0B3-FD3F66826203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="288">
   <si>
     <t>Is Sırası</t>
   </si>
@@ -882,6 +882,9 @@
   </si>
   <si>
     <t>6--12</t>
+  </si>
+  <si>
+    <t>merhaba</t>
   </si>
 </sst>
 </file>
@@ -2417,10 +2420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2691,6 +2694,17 @@
         <v>276</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>287</v>
+      </c>
+      <c r="D14" t="s">
+        <v>287</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
C001- warning hatası almayacak tüm kodlarda summary yazımı yapıldı
</commit_message>
<xml_diff>
--- a/docs/ArchiX_Is_Takip_Listesi.xlsx
+++ b/docs/ArchiX_Is_Takip_Listesi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\ArchiX\notlarim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A4FD80-9F42-4AD1-A4D9-82E4B8CBCD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBA8B40-B528-4F64-8886-19848F2EC454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="287">
   <si>
     <t>Is Sırası</t>
   </si>
@@ -882,12 +882,6 @@
   </si>
   <si>
     <t>6--12</t>
-  </si>
-  <si>
-    <t>deneme</t>
-  </si>
-  <si>
-    <t>****-</t>
   </si>
 </sst>
 </file>
@@ -2423,10 +2417,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2697,20 +2691,6 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>288</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>287</v>
-      </c>
-      <c r="D14" t="s">
-        <v>287</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>